<commit_message>
fixing data file failures
</commit_message>
<xml_diff>
--- a/src/test/resources/data/userData.xlsx
+++ b/src/test/resources/data/userData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>USERNAME</t>
   </si>
@@ -19,31 +19,19 @@
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>MESSAGE</t>
-  </si>
-  <si>
     <t>standard_user</t>
   </si>
   <si>
     <t>secret_sauce</t>
   </si>
   <si>
-    <t>""</t>
-  </si>
-  <si>
     <t>locked_out_user</t>
   </si>
   <si>
-    <t>Epic sadface: Sorry, this user has been locked out.</t>
-  </si>
-  <si>
     <t>hello_world</t>
   </si>
   <si>
     <t>secret_password</t>
-  </si>
-  <si>
-    <t>Epic sadface: Username and password do not match any user in this service</t>
   </si>
 </sst>
 </file>
@@ -302,7 +290,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="18.25"/>
     <col customWidth="1" min="2" max="2" width="17.25"/>
-    <col customWidth="1" min="3" max="3" width="58.88"/>
+    <col customWidth="1" min="3" max="3" width="16.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -312,41 +300,29 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>